<commit_message>
functioning ranking, however, non-functional bonus display
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/19-20/varsity swimmin/isb-varsity-swimming-rankings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD49B1A-BC41-9F42-813B-AD44B4A1A37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8598F6A-D933-3A49-86E8-B5EC95C539A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="500" windowWidth="27640" windowHeight="15940" activeTab="1" xr2:uid="{C577314F-7459-7C40-9827-973F3124A75C}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15940" xr2:uid="{C577314F-7459-7C40-9827-973F3124A75C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Men's" sheetId="1" r:id="rId1"/>
-    <sheet name="Women's" sheetId="2" r:id="rId2"/>
+    <sheet name="MALE" sheetId="1" r:id="rId1"/>
+    <sheet name="FEMALE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -415,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E24A21-58C1-7940-AC26-27B261448AC0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18133547-A8CA-4E4E-A5F3-A1782CB1CFA0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>